<commit_message>
test data name change
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/TestData.xlsx
+++ b/src/test/resources/ExcelFiles/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Framework\src\test\resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya\Desktop\flowapp-web\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61,16 +61,16 @@
     <t>Login Page</t>
   </si>
   <si>
-    <t>Test Data for kATALYST DM WEB PORTAL</t>
-  </si>
-  <si>
-    <t>ProjectID: KATALYST DATA MANAGEMENT</t>
-  </si>
-  <si>
     <t>FLOW_TC_01</t>
   </si>
   <si>
     <t>Create a project and assign task and subscribe the task and check for the catchup funcationality</t>
+  </si>
+  <si>
+    <t>ProjectID:FLOW DATA MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Test Data for FLOW DM WEB PORTAL</t>
   </si>
 </sst>
 </file>
@@ -727,9 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -745,12 +743,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>0</v>
@@ -792,10 +790,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>8</v>

</xml_diff>